<commit_message>
Moji, this is a direct message for you changes performed were to manuscript which is your R Code updates, please review. Also, manuscript has a current date of 07.03.24 which validates the latest update.
</commit_message>
<xml_diff>
--- a/exampledata2MOji.xlsx
+++ b/exampledata2MOji.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{604D9A08-6E43-3D43-BFFC-FF65AF58902C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C53D448B-35CF-4E13-BFE7-1AF5A495EE99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
   <si>
     <t>Height</t>
   </si>
@@ -74,40 +74,31 @@
     <t>identified gender (male/female/other)</t>
   </si>
   <si>
-    <t>Eye color</t>
-  </si>
-  <si>
-    <t>Waist</t>
-  </si>
-  <si>
-    <t>Blue</t>
-  </si>
-  <si>
-    <t>Green</t>
-  </si>
-  <si>
-    <t>Brown</t>
-  </si>
-  <si>
-    <t>Black</t>
-  </si>
-  <si>
-    <t>White</t>
-  </si>
-  <si>
-    <t>Indigo</t>
-  </si>
-  <si>
-    <t>Eye Color</t>
-  </si>
-  <si>
-    <t>Natural eye color</t>
-  </si>
-  <si>
-    <t>Black brown, blue</t>
-  </si>
-  <si>
-    <t>Waist incentimeters</t>
+    <t>Inseam</t>
+  </si>
+  <si>
+    <t>Hair Color</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>blond</t>
+  </si>
+  <si>
+    <t>brown</t>
+  </si>
+  <si>
+    <t>l brown</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>d brown</t>
+  </si>
+  <si>
+    <t>white</t>
   </si>
 </sst>
 </file>
@@ -436,13 +427,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20:F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -459,7 +450,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>180</v>
       </c>
@@ -469,14 +460,14 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2">
+        <v>81</v>
+      </c>
+      <c r="E2" t="s">
         <v>19</v>
       </c>
-      <c r="E2">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>175</v>
       </c>
@@ -486,14 +477,14 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3">
+        <v>74</v>
+      </c>
+      <c r="E3" t="s">
         <v>20</v>
       </c>
-      <c r="E3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -503,14 +494,14 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4">
+        <v>55</v>
+      </c>
+      <c r="E4" t="s">
         <v>21</v>
       </c>
-      <c r="E4">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>178</v>
       </c>
@@ -520,14 +511,14 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>91</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>192</v>
       </c>
@@ -537,14 +528,14 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>95</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -554,14 +545,14 @@
       <c r="C7" t="s">
         <v>4</v>
       </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>89</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>156</v>
       </c>
@@ -571,14 +562,14 @@
       <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>68</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>166</v>
       </c>
@@ -588,14 +579,14 @@
       <c r="C9" t="s">
         <v>3</v>
       </c>
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>62</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>155</v>
       </c>
@@ -605,14 +596,14 @@
       <c r="C10" t="s">
         <v>12</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10">
+        <v>73</v>
+      </c>
+      <c r="E10" t="s">
         <v>21</v>
       </c>
-      <c r="E10">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>145</v>
       </c>
@@ -622,28 +613,28 @@
       <c r="C11" t="s">
         <v>3</v>
       </c>
-      <c r="D11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>49</v>
+      </c>
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>165</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
-      <c r="D12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>53</v>
+      </c>
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>133</v>
       </c>
@@ -653,14 +644,14 @@
       <c r="C13" t="s">
         <v>4</v>
       </c>
-      <c r="D13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>50</v>
+      </c>
+      <c r="E13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>166</v>
       </c>
@@ -670,14 +661,14 @@
       <c r="C14" t="s">
         <v>3</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14">
+        <v>52</v>
+      </c>
+      <c r="E14" t="s">
         <v>24</v>
       </c>
-      <c r="E14">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>154</v>
       </c>
@@ -687,11 +678,11 @@
       <c r="C15" t="s">
         <v>3</v>
       </c>
-      <c r="D15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15">
-        <v>38</v>
+      <c r="D15">
+        <v>65</v>
+      </c>
+      <c r="E15" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -701,20 +692,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A2C8F0-62B4-4D60-B490-D490A3E0B40F}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -725,7 +716,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -736,7 +727,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -747,7 +738,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -756,28 +747,6 @@
       </c>
       <c r="C4" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>